<commit_message>
Add formatting to Excel example
</commit_message>
<xml_diff>
--- a/bw2io/data/examples/example.xlsx
+++ b/bw2io/data/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="28300" windowHeight="20520" activeTab="2"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="28300" windowHeight="20520"/>
   </bookViews>
   <sheets>
     <sheet name="skip this sheet" sheetId="2" r:id="rId1"/>
@@ -617,7 +617,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
@@ -627,17 +629,17 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
     </row>
@@ -656,7 +658,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A22:XFD45"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1014,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix links in example sheet
</commit_message>
<xml_diff>
--- a/bw2io/data/examples/example.xlsx
+++ b/bw2io/data/examples/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="28300" windowHeight="20520"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="28300" windowHeight="20520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="skip this sheet" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="66">
   <si>
     <t>Database</t>
-  </si>
-  <si>
-    <t>BW2 CSV example</t>
   </si>
   <si>
     <t>extracted from</t>
@@ -298,8 +295,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -314,15 +313,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
@@ -625,22 +626,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -657,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -674,13 +675,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1">
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15">
@@ -688,88 +689,88 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15">
       <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -777,87 +778,87 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15">
       <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
         <v>33</v>
       </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
       <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
         <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -866,39 +867,39 @@
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
         <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>36</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -907,39 +908,39 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="J18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -948,39 +949,39 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>0.53900000000000003</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -989,16 +990,16 @@
         <v>0.53900000000000003</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1017,51 +1018,51 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1069,71 +1070,71 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1141,269 +1142,269 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15">
       <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>5.8E-5</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
         <v>35</v>
-      </c>
-      <c r="G23" t="s">
-        <v>36</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>0.53</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
         <v>35</v>
-      </c>
-      <c r="G24" t="s">
-        <v>36</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <v>8.7999999999999998E-5</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
         <v>35</v>
-      </c>
-      <c r="G25" t="s">
-        <v>36</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>8.0499999999999999E-3</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>